<commit_message>
Modificacion Incidencia CNPJ con 11 posiciones
</commit_message>
<xml_diff>
--- a/doc/CAsos de Prueba GEtty Brasil.xlsx
+++ b/doc/CAsos de Prueba GEtty Brasil.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiiselam\Documents\GitHub\br02\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79D716-5B3A-436D-807D-0A0047B618A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5980F0F-42E9-4689-96B9-66587ED07A91}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{77FA00E5-F589-46C3-A1D3-16B2AFE65E68}"/>
   </bookViews>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F3A655-C69E-471C-9B79-556DD9F7A358}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,6 +1569,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="M24:M26"/>
+    <mergeCell ref="N24:N26"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="J15:J23"/>
@@ -1576,11 +1581,6 @@
     <mergeCell ref="M15:M23"/>
     <mergeCell ref="J3:J10"/>
     <mergeCell ref="J11:J13"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="M24:M26"/>
-    <mergeCell ref="N24:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>